<commit_message>
Update out of stock parts
</commit_message>
<xml_diff>
--- a/F405_pill_V1.11/MANUFACTURE/F405_PILL_BOM.xlsx
+++ b/F405_pill_V1.11/MANUFACTURE/F405_PILL_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/owhite/kicad/F405_pill/F405_pill_V1.11/MANUFACTURE/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A447523-2117-1840-92A8-A63D5653537C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D5D8DE8-7388-49E4-8D9B-A28E9F074EF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44700" yWindow="5800" windowWidth="27640" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="F405_PILL_BOM" sheetId="1" r:id="rId1"/>
@@ -133,18 +133,12 @@
     <t>LED_SMD:LED_0603_1608Metric</t>
   </si>
   <si>
-    <t>C72041</t>
-  </si>
-  <si>
     <t>GRN</t>
   </si>
   <si>
     <t>D2</t>
   </si>
   <si>
-    <t>C72043</t>
-  </si>
-  <si>
     <t>RED</t>
   </si>
   <si>
@@ -299,13 +293,19 @@
   </si>
   <si>
     <t>C12084</t>
+  </si>
+  <si>
+    <t>C2689219</t>
+  </si>
+  <si>
+    <t>C87326</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="19">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -793,48 +793,48 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -850,7 +850,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1149,16 +1149,16 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
     <col min="2" max="2" width="47.5" customWidth="1"/>
-    <col min="3" max="3" width="42.6640625" customWidth="1"/>
+    <col min="3" max="3" width="42.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1172,7 +1172,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1186,7 +1186,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1200,7 +1200,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1214,7 +1214,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1225,15 +1225,15 @@
         <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -1242,7 +1242,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1270,7 +1270,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1298,7 +1298,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -1323,217 +1323,217 @@
         <v>36</v>
       </c>
       <c r="D12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
         <v>38</v>
-      </c>
-      <c r="B13" t="s">
-        <v>39</v>
       </c>
       <c r="C13" t="s">
         <v>36</v>
       </c>
       <c r="D13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" t="s">
-        <v>42</v>
       </c>
       <c r="C14" t="s">
         <v>36</v>
       </c>
       <c r="D14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="C15" t="s">
         <v>44</v>
       </c>
-      <c r="B15" t="s">
+      <c r="D15" t="s">
         <v>45</v>
       </c>
-      <c r="C15" t="s">
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
         <v>46</v>
       </c>
-      <c r="D15" t="s">
+      <c r="B16" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="C16" t="s">
         <v>48</v>
       </c>
-      <c r="B16" t="s">
+      <c r="D16" t="s">
         <v>49</v>
       </c>
-      <c r="C16" t="s">
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
         <v>50</v>
       </c>
-      <c r="D16" t="s">
+      <c r="B17" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="C17" t="s">
         <v>52</v>
       </c>
-      <c r="B17" t="s">
+      <c r="D17" t="s">
         <v>53</v>
       </c>
-      <c r="C17" t="s">
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
         <v>54</v>
       </c>
-      <c r="D17" t="s">
+      <c r="B18" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="C18" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" t="s">
         <v>56</v>
       </c>
-      <c r="B18" t="s">
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
         <v>57</v>
       </c>
-      <c r="C18" t="s">
-        <v>54</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="B19" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="C19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" t="s">
         <v>59</v>
       </c>
-      <c r="B19" t="s">
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
         <v>60</v>
       </c>
-      <c r="C19" t="s">
-        <v>54</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="B20" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="C20" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" t="s">
         <v>62</v>
       </c>
-      <c r="B20" t="s">
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
         <v>63</v>
       </c>
-      <c r="C20" t="s">
-        <v>54</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="B21" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="C21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" t="s">
         <v>65</v>
       </c>
-      <c r="B21" t="s">
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
         <v>66</v>
       </c>
-      <c r="C21" t="s">
-        <v>54</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="B22" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="C22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" t="s">
         <v>68</v>
       </c>
-      <c r="B22" t="s">
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
         <v>69</v>
       </c>
-      <c r="C22" t="s">
-        <v>54</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="B23" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="C23" t="s">
         <v>71</v>
       </c>
-      <c r="B23" t="s">
+      <c r="D23" t="s">
         <v>72</v>
       </c>
-      <c r="C23" t="s">
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
         <v>73</v>
       </c>
-      <c r="D23" t="s">
+      <c r="B24" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="C24" t="s">
         <v>75</v>
       </c>
-      <c r="B24" t="s">
+      <c r="D24" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
         <v>76</v>
       </c>
-      <c r="C24" t="s">
+      <c r="B25" t="s">
         <v>77</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="C25" t="s">
         <v>78</v>
       </c>
-      <c r="B25" t="s">
+      <c r="D25" t="s">
         <v>79</v>
       </c>
-      <c r="C25" t="s">
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
         <v>80</v>
       </c>
-      <c r="D25" t="s">
+      <c r="B26" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="C26" t="s">
         <v>82</v>
       </c>
-      <c r="B26" t="s">
+      <c r="D26" t="s">
         <v>83</v>
       </c>
-      <c r="C26" t="s">
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
         <v>84</v>
       </c>
-      <c r="D26" t="s">
+      <c r="B27" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="C27" t="s">
         <v>86</v>
       </c>
-      <c r="B27" t="s">
+      <c r="D27" t="s">
         <v>87</v>
-      </c>
-      <c r="C27" t="s">
-        <v>88</v>
-      </c>
-      <c r="D27" t="s">
-        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>